<commit_message>
Handle time value in Excel cell
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/tableCellsInVariousFormats.xlsx
+++ b/src/test/resources/excel/tableCellsInVariousFormats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB45137C-39CE-9F46-B72D-F45B279FC3FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584A73C3-FDC7-024F-9DE4-694EC03F5E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38820" yWindow="5680" windowWidth="28040" windowHeight="17440" xr2:uid="{54E42A9F-0969-6C4F-8292-50360ADD0D30}"/>
+    <workbookView xWindow="58000" yWindow="14500" windowWidth="28040" windowHeight="17440" xr2:uid="{54E42A9F-0969-6C4F-8292-50360ADD0D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="d\.m\.yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,9 +95,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,7 +437,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +477,21 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="3">
+        <v>45669</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add GRC, WPAFCC and UT_IAC non-strategic list types
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/tableCellsInVariousFormats.xlsx
+++ b/src/test/resources/excel/tableCellsInVariousFormats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584A73C3-FDC7-024F-9DE4-694EC03F5E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0EE25B-96A3-9544-8D67-7BBE5C8AE73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58000" yWindow="14500" windowWidth="28040" windowHeight="17440" xr2:uid="{54E42A9F-0969-6C4F-8292-50360ADD0D30}"/>
+    <workbookView xWindow="58000" yWindow="11520" windowWidth="28040" windowHeight="17440" xr2:uid="{54E42A9F-0969-6C4F-8292-50360ADD0D30}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,13 +50,13 @@
     <t>Boolean</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>10:30am</t>
   </si>
   <si>
     <t>Test string</t>
+  </si>
+  <si>
+    <t>String(s)</t>
   </si>
 </sst>
 </file>
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d\.m\.yy;@"/>
+    <numFmt numFmtId="164" formatCode="d\.m\.yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -99,7 +99,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +437,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -464,7 +464,7 @@
         <v>45668</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>